<commit_message>
Added report and supporting documents
</commit_message>
<xml_diff>
--- a/Bayesian Networks.xlsx
+++ b/Bayesian Networks.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryliu/practices/cs4341/Bayesian-Networks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjnickerson/Documents/WPI/2015-2016/CS/4341/Projects/Bayesian-Networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="4220" windowWidth="31300" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Query1" sheetId="1" r:id="rId1"/>
-    <sheet name="Query2" sheetId="2" r:id="rId2"/>
+    <sheet name="Query1-RS-FINAL" sheetId="3" r:id="rId2"/>
+    <sheet name="Query1-LW-FINAL" sheetId="4" r:id="rId3"/>
+    <sheet name="Query2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t># samples</t>
   </si>
@@ -138,9 +140,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -148,6 +147,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,11 +408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2052680736"/>
-        <c:axId val="-2047034976"/>
+        <c:axId val="-2027177200"/>
+        <c:axId val="-2027171136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2052680736"/>
+        <c:axId val="-2027177200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800.0"/>
@@ -530,12 +532,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047034976"/>
+        <c:crossAx val="-2027171136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2047034976"/>
+        <c:axId val="-2027171136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052680736"/>
+        <c:crossAx val="-2027177200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -973,11 +975,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2072302400"/>
-        <c:axId val="-2054432944"/>
+        <c:axId val="-2027863936"/>
+        <c:axId val="-2027885248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2072302400"/>
+        <c:axId val="-2027863936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800.0"/>
@@ -1097,12 +1099,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054432944"/>
+        <c:crossAx val="-2027885248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2054432944"/>
+        <c:axId val="-2027885248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,7 +1217,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072302400"/>
+        <c:crossAx val="-2027863936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1337,7 +1339,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1541,11 +1542,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2072628448"/>
-        <c:axId val="-2074922176"/>
+        <c:axId val="-2026038832"/>
+        <c:axId val="-2026798672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2072628448"/>
+        <c:axId val="-2026038832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800.0"/>
@@ -1598,7 +1599,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1665,12 +1665,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074922176"/>
+        <c:crossAx val="-2026798672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2074922176"/>
+        <c:axId val="-2026798672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,7 +1716,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1783,7 +1782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072628448"/>
+        <c:crossAx val="-2026038832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1797,7 +1796,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1904,7 +1902,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2108,11 +2105,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2075548848"/>
-        <c:axId val="2145590080"/>
+        <c:axId val="-2028225440"/>
+        <c:axId val="-2028229232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2075548848"/>
+        <c:axId val="-2028225440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800.0"/>
@@ -2165,7 +2162,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2232,12 +2228,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145590080"/>
+        <c:crossAx val="-2028229232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145590080"/>
+        <c:axId val="-2028229232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2283,7 +2279,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2350,7 +2345,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2075548848"/>
+        <c:crossAx val="-2028225440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2364,7 +2359,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5056,8 +5050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5110,7 +5104,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
@@ -5156,7 +5150,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3">
         <v>400</v>
       </c>
@@ -5200,7 +5194,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3">
         <v>600</v>
       </c>
@@ -5244,7 +5238,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3">
         <v>800</v>
       </c>
@@ -5269,7 +5263,7 @@
       <c r="I5" s="3">
         <v>0.461538</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>0.34482800000000002</v>
       </c>
       <c r="K5" s="3">
@@ -5288,7 +5282,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3">
         <v>1000</v>
       </c>
@@ -5332,7 +5326,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -5378,7 +5372,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3">
         <v>400</v>
       </c>
@@ -5422,7 +5416,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3">
         <v>600</v>
       </c>
@@ -5447,7 +5441,7 @@
       <c r="I9" s="3">
         <v>0.39632800000000001</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>0.38391900000000001</v>
       </c>
       <c r="K9" s="3">
@@ -5466,7 +5460,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3">
         <v>800</v>
       </c>
@@ -5510,38 +5504,38 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6">
         <v>1000</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0.41954200000000003</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>0.36796400000000001</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>0.39654200000000001</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>0.36226900000000001</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>0.37507200000000002</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>0.37394500000000003</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>0.39675100000000002</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>0.39779100000000001</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>0.38597900000000002</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>0.37858599999999998</v>
       </c>
       <c r="M11" s="1">
@@ -5568,6 +5562,318 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>200</v>
+      </c>
+      <c r="C2" s="3">
+        <v>400</v>
+      </c>
+      <c r="D2" s="3">
+        <v>600</v>
+      </c>
+      <c r="E2" s="3">
+        <v>800</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.31578899999999999</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.31034499999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.40740700000000002</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.44117600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.25806499999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.13636400000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.290323</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.42857099999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.214286</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.47826099999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.37142900000000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.189189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.15151500000000001</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.37930999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.23333300000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.263158</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.43902400000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.461538</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.41025600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.538462</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.34482800000000002</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.55632000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.111111</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.40540500000000002</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.43902400000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.55555600000000005</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.38095200000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.44444400000000001</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.41666700000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE(B3:B12)</f>
+        <v>0.37162709999999999</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C3:C12)</f>
+        <v>0.44534579999999996</v>
+      </c>
+      <c r="D13" s="1">
+        <f>AVERAGE(D3:D12)</f>
+        <v>0.34183020000000008</v>
+      </c>
+      <c r="E13" s="1">
+        <f>AVERAGE(E3:E12)</f>
+        <v>0.33981120000000004</v>
+      </c>
+      <c r="F13" s="1">
+        <f>AVERAGE(F3:F12)</f>
+        <v>0.40495369999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <f>_xlfn.VAR.S(B3:B12)</f>
+        <v>3.5072227380988891E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f>_xlfn.VAR.S(C3:C12)</f>
+        <v>2.5413260826622281E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <f>_xlfn.VAR.S(D3:D12)</f>
+        <v>1.4030664577733325E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>_xlfn.VAR.S(E3:E12)</f>
+        <v>9.5694137963999726E-3</v>
+      </c>
+      <c r="F14" s="1">
+        <f>_xlfn.VAR.S(F3:F12)</f>
+        <v>8.6111543753444562E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5613,15 +5919,15 @@
       <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -5667,7 +5973,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1">
         <v>400</v>
       </c>
@@ -5689,7 +5995,7 @@
       <c r="H3" s="1">
         <v>0.52381</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>0.56115099999999996</v>
       </c>
       <c r="J3" s="1">
@@ -5711,7 +6017,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1">
         <v>600</v>
       </c>
@@ -5755,7 +6061,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1">
         <v>800</v>
       </c>
@@ -5774,7 +6080,7 @@
       <c r="G5" s="1">
         <v>0.43442599999999998</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0.48262500000000003</v>
       </c>
       <c r="I5" s="1">
@@ -5799,8 +6105,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9">
+      <c r="A6" s="9"/>
+      <c r="B6" s="8">
         <v>1000</v>
       </c>
       <c r="C6" s="1">
@@ -5843,7 +6149,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1">
@@ -5889,7 +6195,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1">
         <v>400</v>
       </c>
@@ -5933,7 +6239,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1">
         <v>600</v>
       </c>
@@ -5977,38 +6283,38 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1">
         <v>800</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>0.46250000000000002</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.50375000000000003</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.47499999999999998</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.45874999999999999</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0.48499999999999999</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>0.5</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>0.50124999999999997</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>0.47499999999999998</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>0.49625000000000002</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="8">
         <v>0.47625000000000001</v>
       </c>
       <c r="M10" s="1">
@@ -6021,38 +6327,38 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8">
         <v>1000</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>0.49199999999999999</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.49199999999999999</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>0.48599999999999999</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.49199999999999999</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0.502</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>0.47799999999999998</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>0.48299999999999998</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>0.46800000000000003</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="8">
         <v>0.48699999999999999</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>0.497</v>
       </c>
       <c r="M11" s="1">

</xml_diff>